<commit_message>
May 11th 2020 v2
</commit_message>
<xml_diff>
--- a/LockDownMaps_200511_EU.xlsx
+++ b/LockDownMaps_200511_EU.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
   <si>
     <t xml:space="preserve">Coronavirus Lockdown Maps companion</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Released under GNU Licence v3 by RafDouglas C. Tommasi – 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Updated 11/05/2020 v1</t>
+    <t xml:space="preserve">Updated 11/05/2020 v2</t>
   </si>
   <si>
     <t xml:space="preserve">Not published on map</t>
@@ -169,6 +169,9 @@
     <t xml:space="preserve">France</t>
   </si>
   <si>
+    <t xml:space="preserve">Some schools reopened</t>
+  </si>
+  <si>
     <t xml:space="preserve">relaxing of lockdown</t>
   </si>
   <si>
@@ -283,6 +286,9 @@
     <t xml:space="preserve">Sport an walking outside is allowed, Barcelona and Madrid still in Phase 0 lockdown</t>
   </si>
   <si>
+    <t xml:space="preserve">Max 10 people in some parts of the Country</t>
+  </si>
+  <si>
     <t xml:space="preserve">Restaurants and bars limited reopening</t>
   </si>
   <si>
@@ -404,15 +410,17 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.theguardian.com/world/2020/may/11/lockdown-easing-have-other-leaders-fared-better-than-boris-johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.nytimes.com/2020/05/11/world/coronavirus-news.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -808,18 +816,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -895,10 +903,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topRight" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.73"/>
@@ -916,6 +924,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="13.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="13.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="32" style="0" width="13.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="35" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,11 +1580,11 @@
         <v>46</v>
       </c>
       <c r="C20" s="32" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D20" s="33"/>
       <c r="E20" s="34" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F20" s="32" t="n">
         <v>1</v>
@@ -1585,11 +1594,13 @@
         <v>2</v>
       </c>
       <c r="I20" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J20" s="33"/>
+        <v>0.75</v>
+      </c>
+      <c r="J20" s="33" t="s">
+        <v>47</v>
+      </c>
       <c r="K20" s="33" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="L20" s="32" t="n">
         <v>0</v>
@@ -1608,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AC20" s="35"/>
       <c r="AD20" s="18"/>
@@ -1624,13 +1635,13 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31"/>
       <c r="B21" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="32" t="n">
         <v>0.25</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E21" s="34" t="n">
         <v>20.2</v>
@@ -1639,7 +1650,7 @@
         <v>0.5</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H21" s="34" t="n">
         <v>20</v>
@@ -1648,7 +1659,7 @@
         <v>0.5</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K21" s="33" t="n">
         <v>5</v>
@@ -1657,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N21" s="34" t="n">
         <v>19</v>
@@ -1666,22 +1677,22 @@
         <v>1</v>
       </c>
       <c r="P21" s="33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q21" s="33" t="n">
         <v>2</v>
       </c>
       <c r="U21" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="V21" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AC21" s="38" t="n">
         <v>0.5</v>
       </c>
       <c r="AD21" s="37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AE21" s="39" t="n">
         <v>2</v>
@@ -1695,7 +1706,7 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="31"/>
       <c r="B22" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>1</v>
@@ -1718,7 +1729,7 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31"/>
       <c r="B23" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>1</v>
@@ -1730,7 +1741,7 @@
         <v>0.5</v>
       </c>
       <c r="M23" s="33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N23" s="34" t="n">
         <v>2</v>
@@ -1754,7 +1765,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31"/>
       <c r="B24" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C24" s="32" t="n">
         <v>1</v>
@@ -1788,13 +1799,13 @@
         <v>0.75</v>
       </c>
       <c r="P24" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q24" s="33" t="n">
         <v>2</v>
       </c>
       <c r="V24" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AC24" s="35"/>
       <c r="AD24" s="18"/>
@@ -1810,13 +1821,13 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="31"/>
       <c r="B25" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C25" s="32" t="n">
         <v>0.5</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E25" s="34"/>
       <c r="F25" s="32" t="n">
@@ -1833,14 +1844,14 @@
         <v>1</v>
       </c>
       <c r="M25" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N25" s="34"/>
       <c r="O25" s="33" t="n">
         <v>0.75</v>
       </c>
       <c r="P25" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q25" s="33"/>
       <c r="AC25" s="38" t="n">
@@ -1857,7 +1868,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="31"/>
       <c r="B26" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC26" s="35"/>
       <c r="AD26" s="18"/>
@@ -1869,7 +1880,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="31"/>
       <c r="B27" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AC27" s="35"/>
       <c r="AD27" s="18"/>
@@ -1881,7 +1892,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="31"/>
       <c r="B28" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AC28" s="35"/>
       <c r="AD28" s="18"/>
@@ -1893,7 +1904,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="31"/>
       <c r="B29" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC29" s="35"/>
       <c r="AD29" s="18"/>
@@ -1905,7 +1916,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="31"/>
       <c r="B30" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C30" s="32" t="n">
         <v>0.25</v>
@@ -1918,7 +1929,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H30" s="34" t="n">
         <v>7</v>
@@ -1927,7 +1938,7 @@
         <v>0.5</v>
       </c>
       <c r="J30" s="33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K30" s="34" t="n">
         <v>7</v>
@@ -1936,7 +1947,7 @@
         <v>0.25</v>
       </c>
       <c r="M30" s="33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N30" s="34" t="n">
         <v>7</v>
@@ -1949,7 +1960,7 @@
         <v>7</v>
       </c>
       <c r="X30" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC30" s="35"/>
       <c r="AD30" s="18"/>
@@ -1958,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="AG30" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AH30" s="18" t="n">
         <v>7</v>
@@ -1967,13 +1978,13 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="31"/>
       <c r="B31" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C31" s="32" t="n">
         <v>0.25</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E31" s="34" t="n">
         <v>2</v>
@@ -1982,7 +1993,7 @@
         <v>0.25</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H31" s="33" t="n">
         <v>22</v>
@@ -1991,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K31" s="33" t="n">
         <v>2</v>
@@ -2000,7 +2011,7 @@
         <v>0.25</v>
       </c>
       <c r="M31" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N31" s="34" t="n">
         <v>2</v>
@@ -2009,7 +2020,7 @@
         <v>0.75</v>
       </c>
       <c r="P31" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q31" s="33" t="n">
         <v>22</v>
@@ -2024,7 +2035,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="31"/>
       <c r="B32" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>1</v>
@@ -2045,7 +2056,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="31"/>
       <c r="B33" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AC33" s="35"/>
       <c r="AD33" s="18"/>
@@ -2057,7 +2068,7 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="31"/>
       <c r="B34" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AC34" s="35"/>
       <c r="AD34" s="18"/>
@@ -2069,7 +2080,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="31"/>
       <c r="B35" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AC35" s="35"/>
       <c r="AD35" s="18"/>
@@ -2081,23 +2092,25 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="31"/>
       <c r="B36" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36" s="32" t="n">
         <v>0.5</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E36" s="34" t="n">
         <v>17.2</v>
       </c>
       <c r="F36" s="32" t="n">
-        <v>1</v>
-      </c>
-      <c r="G36" s="33"/>
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>86</v>
+      </c>
       <c r="H36" s="34" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>1</v>
@@ -2106,7 +2119,7 @@
         <v>0.5</v>
       </c>
       <c r="M36" s="33" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N36" s="33" t="n">
         <v>2</v>
@@ -2115,7 +2128,7 @@
         <v>0.5</v>
       </c>
       <c r="P36" s="33" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Q36" s="33" t="n">
         <v>2</v>
@@ -2124,7 +2137,7 @@
         <v>0.75</v>
       </c>
       <c r="AD36" s="37" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AE36" s="39" t="n">
         <v>2</v>
@@ -2140,13 +2153,13 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="31"/>
       <c r="B37" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C37" s="32" t="n">
         <v>0.75</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E37" s="34" t="n">
         <v>2</v>
@@ -2164,7 +2177,7 @@
         <v>0.75</v>
       </c>
       <c r="J37" s="33" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K37" s="33" t="n">
         <v>11</v>
@@ -2184,7 +2197,7 @@
         <v>10</v>
       </c>
       <c r="X37" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AC37" s="38" t="n">
         <v>0.5</v>
@@ -2202,7 +2215,7 @@
     <row r="38" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="31"/>
       <c r="B38" s="30" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C38" s="40" t="n">
         <v>0</v>
@@ -2213,7 +2226,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H38" s="42" t="n">
         <v>2</v>
@@ -2222,7 +2235,7 @@
         <v>0.5</v>
       </c>
       <c r="J38" s="41" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K38" s="41" t="n">
         <v>2</v>
@@ -2300,28 +2313,29 @@
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="191.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="47" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="47" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2332,17 +2346,17 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="46" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="48" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="47" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2357,7 +2371,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,16 +2418,16 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="49" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B27" s="49"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="50" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,10 +2447,10 @@
         <v>2</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,7 +2458,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2452,7 +2466,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,7 +2474,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,7 +2482,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="47" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2476,7 +2490,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2498,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="47" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,7 +2506,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="47" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,7 +2514,7 @@
         <v>10</v>
       </c>
       <c r="B39" s="47" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,7 +2522,7 @@
         <v>11</v>
       </c>
       <c r="B40" s="47" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,7 +2530,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="47" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,7 +2538,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,7 +2546,7 @@
         <v>14</v>
       </c>
       <c r="B43" s="47" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2540,7 +2554,7 @@
         <v>15</v>
       </c>
       <c r="B44" s="47" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,7 +2562,7 @@
         <v>16</v>
       </c>
       <c r="B45" s="47" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,7 +2570,7 @@
         <v>17</v>
       </c>
       <c r="B46" s="47" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2564,7 +2578,7 @@
         <v>18</v>
       </c>
       <c r="B47" s="47" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2586,7 @@
         <v>19</v>
       </c>
       <c r="B48" s="47" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,7 +2594,7 @@
         <v>20</v>
       </c>
       <c r="B49" s="47" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2588,7 +2602,7 @@
         <v>21</v>
       </c>
       <c r="B50" s="47" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2596,7 +2610,7 @@
         <v>22</v>
       </c>
       <c r="B51" s="47" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,7 +2618,7 @@
         <v>23</v>
       </c>
       <c r="B52" s="47" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,12 +2626,16 @@
         <v>24</v>
       </c>
       <c r="B53" s="47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="51"/>
-      <c r="B54" s="47"/>
+      <c r="A54" s="51" t="n">
+        <v>25</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="51"/>
@@ -2740,10 +2758,12 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2879,7 +2899,7 @@
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">IF(LEN(_Data!C20)=0,"",_Data!C20)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">IF(LEN(_Data!D20)=0,"",_Data!D20)</f>
@@ -3160,10 +3180,12 @@
       <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,11 +3545,11 @@
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">IF(LEN(_Data!F36)=0,"",_Data!F36)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C26" s="0" t="str">
         <f aca="false">IF(LEN(_Data!G36)=0,"",_Data!G36)</f>
-        <v/>
+        <v>Max 10 people in some parts of the Country</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,10 +3602,12 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3719,11 +3743,11 @@
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">IF(LEN(_Data!I20)=0,"",_Data!I20)</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">IF(LEN(_Data!J20)=0,"",_Data!J20)</f>
-        <v/>
+        <v>Some schools reopened</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4000,10 +4024,12 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4420,10 +4446,12 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>